<commit_message>
sources without inputs working
</commit_message>
<xml_diff>
--- a/project/excel/shareyourcloning_linkml.xlsx
+++ b/project/excel/shareyourcloning_linkml.xlsx
@@ -8,8 +8,10 @@
   </bookViews>
   <sheets>
     <sheet name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="CloningStrategy" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="CloningStrategyCollection" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="ManuallyTypedSource" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="UploadedFileSource" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="RepositoryIdSource" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="GenomeCoordinatesSource" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -415,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -427,16 +429,6 @@
       <c r="A1" t="inlineStr">
         <is>
           <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
         </is>
       </c>
     </row>
@@ -462,44 +454,44 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>primary_email</t>
+          <t>user_input</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>birth_date</t>
+          <t>input</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>age_in_years</t>
+          <t>output</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>vital_status</t>
+          <t>type</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>kind</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>info</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>id</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>description</t>
         </is>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ALIVE,DEAD,UNKNOWN"</formula1>
+      <formula1>"repository_id,file,restriction,ligation,PCR,homologous_recombination,gibson_assembly,restriction_and_ligation,genome_coordinates,manually_typed"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -512,7 +504,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -523,11 +515,211 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>entries</t>
+          <t>file_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>index_in_file</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>kind</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>info</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>id</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"repository_id,file,restriction,ligation,PCR,homologous_recombination,gibson_assembly,restriction_and_ligation,genome_coordinates,manually_typed"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>repository_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>repository_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>kind</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>info</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"addgene,genbank"</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"repository_id,file,restriction,ligation,PCR,homologous_recombination,gibson_assembly,restriction_and_ligation,genome_coordinates,manually_typed"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>assembly_accession</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sequence_accession</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>locus_tag</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>gene_id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>start</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>stop</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>strand</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>kind</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>info</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="J2:J1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"repository_id,file,restriction,ligation,PCR,homologous_recombination,gibson_assembly,restriction_and_ligation,genome_coordinates,manually_typed"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
working version, prior to try pypi
</commit_message>
<xml_diff>
--- a/project/excel/shareyourcloning_linkml.xlsx
+++ b/project/excel/shareyourcloning_linkml.xlsx
@@ -8,17 +8,27 @@
   </bookViews>
   <sheets>
     <sheet name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="CloningStrategy" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="TextFileSequence" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Primer" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="SequenceCut" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="RestrictionSequenceCut" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="ManuallyTypedSource" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="UploadedFileSource" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="RepositoryIdSource" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="GenomeCoordinatesSource" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="CutSource" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="RestrictionCutSource" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="TextFileSequence" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Primer" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="SequenceCut" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="RestrictionSequenceCut" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="ManuallyTypedSource" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="UploadedFileSource" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="RepositoryIdSource" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="GenomeCoordinatesSource" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="SequenceCutSource" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="RestrictionEnzymeDigestionSource" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="SimpleSequenceLocation" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="AssemblyJoin" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="AssemblySource" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="PCRSource" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="LigationSource" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="HomologousRecombinationSource" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="GibsonAssemblySource" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="RestrictionAndLigationSource" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="OligoHybridizationSource" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="PolymeraseExtensionSource" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="CloningStrategy" sheetId="22" state="visible" r:id="rId22"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -450,77 +460,343 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>assembly_accession</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sequence_accession</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>locus_tag</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>gene_id</t>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>left_edge</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>right_edge</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>left_edge</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>right_edge</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>start</t>
         </is>
       </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>end</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>strand</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>left_fragment</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>right_fragment</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>left_location</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>right_location</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>assembly</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>stop</t>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>forward_primer</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>reverse_primer</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>assembly</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>output</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>strand</t>
+          <t>type</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>assembly</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>input</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>output</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>type</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -537,12 +813,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>left_cut</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>right_cut</t>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>assembly</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -571,7 +847,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -588,12 +864,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>left_cut</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>right_cut</t>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>assembly</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -622,48 +898,63 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>restriction_enzymes</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>assembly</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sequences</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sources</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>primers</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -719,12 +1010,222 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>forward_oligo</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>reverse_oligo</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>overhang_crick_3prime</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sequences</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sources</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>primers</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sequence</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>cut_watson</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>overhang</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -736,55 +1237,19 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>sequence</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+          <t>restriction_enzyme</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
         <is>
           <t>cut_watson</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>overhang</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -797,31 +1262,41 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>restriction_enzyme</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>cut_watson</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>overhang</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>user_input</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -833,52 +1308,6 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>user_input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -939,7 +1368,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -993,4 +1422,80 @@
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>assembly_accession</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sequence_accession</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>locus_tag</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>gene_id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>start</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>end</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>strand</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add extra slots to manually typed
</commit_message>
<xml_diff>
--- a/project/excel/shareyourcloning_linkml.xlsx
+++ b/project/excel/shareyourcloning_linkml.xlsx
@@ -976,17 +976,17 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>overhang_crick_3prime</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>overhang_watson_3prime</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>file_content</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>overhang_crick_3prime</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>overhang_watson_3prime</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -1027,276 +1027,286 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>overhang_crick_3prime</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>forward_oligo</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>reverse_oligo</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sequences</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sources</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>primers</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sequence</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>cut_watson</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>overhang</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>restriction_enzyme</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>cut_watson</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>overhang</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
         <is>
           <t>overhang_crick_3prime</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>overhang_watson_3prime</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>user_input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
         <is>
           <t>input</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>output</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>type</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sequences</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sources</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>primers</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sequence</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>cut_watson</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>overhang</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>restriction_enzyme</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>cut_watson</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>overhang</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>user_input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>circular</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>id</t>
         </is>

</xml_diff>

<commit_message>
extra work for https://github.com/manulera/ShareYourCloning_backend/issues/123
</commit_message>
<xml_diff>
--- a/project/excel/shareyourcloning_linkml.xlsx
+++ b/project/excel/shareyourcloning_linkml.xlsx
@@ -15,20 +15,22 @@
     <sheet name="ManuallyTypedSource" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="UploadedFileSource" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="RepositoryIdSource" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="GenomeCoordinatesSource" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="SequenceCutSource" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="RestrictionEnzymeDigestionSource" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="SimpleSequenceLocation" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="AssemblyJoin" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="AssemblySource" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="PCRSource" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="LigationSource" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="HomologousRecombinationSource" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="GibsonAssemblySource" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="RestrictionAndLigationSource" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="OligoHybridizationSource" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="PolymeraseExtensionSource" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="CloningStrategy" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="AddGeneIdSource" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="GenomeCoordinatesSource" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="SequenceCutSource" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="RestrictionEnzymeDigestionSource" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="SimpleSequenceLocation" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="AssemblyJoin" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="AssemblySource" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="PCRSource" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="LigationSource" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="HomologousRecombinationSource" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="GibsonAssemblySource" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="RestrictionAndLigationSource" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="CRISPRSource" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="OligoHybridizationSource" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="PolymeraseExtensionSource" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="CloningStrategy" sheetId="24" state="visible" r:id="rId24"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -460,6 +462,82 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>assembly_accession</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sequence_accession</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>locus_tag</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>gene_id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>start</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>end</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>strand</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -505,7 +583,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -556,7 +634,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -592,7 +670,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -633,7 +711,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -684,7 +762,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -745,7 +823,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -796,7 +874,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -847,7 +925,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -888,62 +966,6 @@
         </is>
       </c>
       <c r="F1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>restriction_enzymes</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>circular</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>assembly</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -1027,6 +1049,118 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>restriction_enzymes</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>assembly</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>guides</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>assembly</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>overhang_crick_3prime</t>
         </is>
       </c>
@@ -1066,7 +1200,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1107,7 +1241,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1440,72 +1574,65 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>assembly_accession</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sequence_accession</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>locus_tag</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>gene_id</t>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sequence_file_url</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>addgene_sequence_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>repository_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>repository_id</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>start</t>
+          <t>input</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>end</t>
+          <t>output</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>strand</t>
+          <t>type</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"depositor-full,addgene-full"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"addgene,genbank"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add circularise to UploadedFileSource + embl as format
</commit_message>
<xml_diff>
--- a/project/excel/shareyourcloning_linkml.xlsx
+++ b/project/excel/shareyourcloning_linkml.xlsx
@@ -1,37 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="TextFileSequence" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Primer" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="SequenceCut" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="RestrictionSequenceCut" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="ManuallyTypedSource" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="UploadedFileSource" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="RepositoryIdSource" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="AddGeneIdSource" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="GenomeCoordinatesSource" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="SequenceCutSource" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="RestrictionEnzymeDigestionSource" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="SimpleSequenceLocation" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="AssemblyJoinComponent" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="AssemblyJoin" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="AssemblySource" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="PCRSource" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="LigationSource" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="HomologousRecombinationSource" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="GibsonAssemblySource" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="RestrictionAndLigationSource" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="CRISPRSource" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="OligoHybridizationSource" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="PolymeraseExtensionSource" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="CloningStrategy" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TextFileSequence" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Primer" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SequenceCut" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RestrictionSequenceCut" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ManuallyTypedSource" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UploadedFileSource" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RepositoryIdSource" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AddGeneIdSource" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GenomeCoordinatesSource" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SequenceCutSource" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RestrictionEnzymeDigestionSource" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SimpleSequenceLocation" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AssemblyJoinComponent" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AssemblyJoin" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AssemblySource" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PCRSource" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LigationSource" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HomologousRecombinationSource" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GibsonAssemblySource" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RestrictionAndLigationSource" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CRISPRSource" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="OligoHybridizationSource" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PolymeraseExtensionSource" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CloningStrategy" sheetId="25" state="visible" r:id="rId25"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1001,7 +1001,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"fasta,genbank,snapgene"</formula1>
+      <formula1>"fasta,genbank,snapgene,embl"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1484,7 +1484,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1510,20 +1510,25 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>circularise</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>input</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>output</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
       <c r="G1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -1532,7 +1537,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"fasta,genbank,snapgene"</formula1>
+      <formula1>"fasta,genbank,snapgene,embl"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add name to sequence class
</commit_message>
<xml_diff>
--- a/project/excel/shareyourcloning_linkml.xlsx
+++ b/project/excel/shareyourcloning_linkml.xlsx
@@ -1,37 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TextFileSequence" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Primer" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SequenceCut" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RestrictionSequenceCut" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ManuallyTypedSource" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UploadedFileSource" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RepositoryIdSource" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AddGeneIdSource" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GenomeCoordinatesSource" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SequenceCutSource" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RestrictionEnzymeDigestionSource" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SimpleSequenceLocation" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AssemblyJoinComponent" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AssemblyJoin" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AssemblySource" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PCRSource" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LigationSource" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HomologousRecombinationSource" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GibsonAssemblySource" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RestrictionAndLigationSource" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CRISPRSource" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="OligoHybridizationSource" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PolymeraseExtensionSource" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CloningStrategy" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="TextFileSequence" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Primer" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="SequenceCut" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="RestrictionSequenceCut" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="ManuallyTypedSource" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="UploadedFileSource" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="RepositoryIdSource" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="AddGeneIdSource" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="GenomeCoordinatesSource" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="SequenceCutSource" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="RestrictionEnzymeDigestionSource" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="SimpleSequenceLocation" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="AssemblyJoinComponent" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="AssemblyJoin" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="AssemblySource" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="PCRSource" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="LigationSource" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="HomologousRecombinationSource" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="GibsonAssemblySource" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="RestrictionAndLigationSource" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="CRISPRSource" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="OligoHybridizationSource" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="PolymeraseExtensionSource" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="CloningStrategy" sheetId="25" state="visible" r:id="rId25"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -958,7 +958,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -995,6 +995,11 @@
       <c r="F1" t="inlineStr">
         <is>
           <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>name</t>
         </is>
       </c>
     </row>
@@ -1326,22 +1331,22 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>sequence</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sequence</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>type</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add name to sequence class (#9)
</commit_message>
<xml_diff>
--- a/project/excel/shareyourcloning_linkml.xlsx
+++ b/project/excel/shareyourcloning_linkml.xlsx
@@ -1,37 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TextFileSequence" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Primer" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SequenceCut" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RestrictionSequenceCut" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ManuallyTypedSource" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UploadedFileSource" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RepositoryIdSource" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AddGeneIdSource" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GenomeCoordinatesSource" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SequenceCutSource" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RestrictionEnzymeDigestionSource" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SimpleSequenceLocation" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AssemblyJoinComponent" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AssemblyJoin" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AssemblySource" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PCRSource" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LigationSource" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HomologousRecombinationSource" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GibsonAssemblySource" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RestrictionAndLigationSource" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CRISPRSource" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="OligoHybridizationSource" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PolymeraseExtensionSource" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CloningStrategy" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="TextFileSequence" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Primer" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="SequenceCut" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="RestrictionSequenceCut" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="ManuallyTypedSource" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="UploadedFileSource" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="RepositoryIdSource" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="AddGeneIdSource" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="GenomeCoordinatesSource" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="SequenceCutSource" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="RestrictionEnzymeDigestionSource" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="SimpleSequenceLocation" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="AssemblyJoinComponent" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="AssemblyJoin" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="AssemblySource" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="PCRSource" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="LigationSource" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="HomologousRecombinationSource" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="GibsonAssemblySource" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="RestrictionAndLigationSource" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="CRISPRSource" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="OligoHybridizationSource" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="PolymeraseExtensionSource" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="CloningStrategy" sheetId="25" state="visible" r:id="rId25"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -958,7 +958,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -995,6 +995,11 @@
       <c r="F1" t="inlineStr">
         <is>
           <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>name</t>
         </is>
       </c>
     </row>
@@ -1326,22 +1331,22 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>sequence</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sequence</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>type</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove name from sequence, and add output_name to source
</commit_message>
<xml_diff>
--- a/project/excel/shareyourcloning_linkml.xlsx
+++ b/project/excel/shareyourcloning_linkml.xlsx
@@ -958,7 +958,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -995,11 +995,6 @@
       <c r="F1" t="inlineStr">
         <is>
           <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>name</t>
         </is>
       </c>
     </row>
@@ -1331,22 +1326,22 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>sequence</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>name</t>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>type</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove name from sequence, and add output_name to source (#10)
</commit_message>
<xml_diff>
--- a/project/excel/shareyourcloning_linkml.xlsx
+++ b/project/excel/shareyourcloning_linkml.xlsx
@@ -958,7 +958,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -995,11 +995,6 @@
       <c r="F1" t="inlineStr">
         <is>
           <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>name</t>
         </is>
       </c>
     </row>
@@ -1331,22 +1326,22 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>sequence</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>name</t>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>type</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove name from sequence, and add output_name to source (#11)
</commit_message>
<xml_diff>
--- a/project/excel/shareyourcloning_linkml.xlsx
+++ b/project/excel/shareyourcloning_linkml.xlsx
@@ -463,7 +463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,6 +524,11 @@
       </c>
       <c r="K1" t="inlineStr">
         <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
@@ -539,7 +544,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -575,6 +580,11 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
@@ -590,7 +600,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -626,6 +636,11 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
@@ -744,7 +759,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -780,6 +795,11 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
@@ -795,7 +815,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -841,6 +861,11 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
@@ -856,7 +881,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -892,6 +917,11 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
@@ -907,7 +937,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -942,6 +972,11 @@
         </is>
       </c>
       <c r="F1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -1014,7 +1049,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1050,6 +1085,11 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
@@ -1065,7 +1105,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1106,6 +1146,11 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
@@ -1121,7 +1166,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1162,6 +1207,11 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
@@ -1177,7 +1227,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1218,6 +1268,11 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
@@ -1233,6 +1288,52 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1244,291 +1345,260 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>sequences</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sources</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>primers</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sequence</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>cut_watson</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>overhang</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>restriction_enzyme</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>cut_watson</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>overhang</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>overhang_crick_3prime</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>overhang_watson_3prime</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>user_input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>input</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>output</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>type</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sequences</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sources</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>primers</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sequence</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sequence_file_format</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>file_name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>index_in_file</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>circularize</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
         <is>
           <t>type</t>
         </is>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>cut_watson</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>overhang</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>restriction_enzyme</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>cut_watson</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>overhang</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>overhang_crick_3prime</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>overhang_watson_3prime</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>user_input</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>circular</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sequence_file_format</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>file_name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>index_in_file</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>circularize</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -1550,7 +1620,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1585,6 +1655,11 @@
         </is>
       </c>
       <c r="F1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -1606,7 +1681,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1651,6 +1726,11 @@
         </is>
       </c>
       <c r="H1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
         <is>
           <t>id</t>
         </is>

</xml_diff>

<commit_message>
support for benchling ids as inputs
</commit_message>
<xml_diff>
--- a/project/excel/shareyourcloning_linkml.xlsx
+++ b/project/excel/shareyourcloning_linkml.xlsx
@@ -1,37 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="TextFileSequence" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Primer" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="SequenceCut" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="RestrictionSequenceCut" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="ManuallyTypedSource" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="UploadedFileSource" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="RepositoryIdSource" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="AddGeneIdSource" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="GenomeCoordinatesSource" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="SequenceCutSource" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="RestrictionEnzymeDigestionSource" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="SimpleSequenceLocation" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="AssemblyJoinComponent" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="AssemblyJoin" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="AssemblySource" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="PCRSource" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="LigationSource" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="HomologousRecombinationSource" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="GibsonAssemblySource" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="RestrictionAndLigationSource" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="CRISPRSource" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="OligoHybridizationSource" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="PolymeraseExtensionSource" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="CloningStrategy" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TextFileSequence" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Primer" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SequenceCut" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RestrictionSequenceCut" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ManuallyTypedSource" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UploadedFileSource" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RepositoryIdSource" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AddGeneIdSource" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BenchlingUrlSource" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GenomeCoordinatesSource" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SequenceCutSource" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RestrictionEnzymeDigestionSource" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SimpleSequenceLocation" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AssemblyJoinComponent" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AssemblyJoin" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AssemblySource" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PCRSource" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LigationSource" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HomologousRecombinationSource" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GibsonAssemblySource" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RestrictionAndLigationSource" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CRISPRSource" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="OligoHybridizationSource" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PolymeraseExtensionSource" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CloningStrategy" sheetId="26" state="visible" r:id="rId26"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -463,6 +464,67 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>repository_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>repository_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"addgene,genbank"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -538,7 +600,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -594,7 +656,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -650,7 +712,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -686,7 +748,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -722,7 +784,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -753,7 +815,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -809,7 +871,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -865,62 +927,6 @@
         </is>
       </c>
       <c r="I1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>circular</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>assembly</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -1105,6 +1111,62 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>assembly</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1160,7 +1222,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1221,7 +1283,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1282,7 +1344,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1328,7 +1390,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
include benchling as type of repository
</commit_message>
<xml_diff>
--- a/project/excel/shareyourcloning_linkml.xlsx
+++ b/project/excel/shareyourcloning_linkml.xlsx
@@ -512,7 +512,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank"</formula1>
+      <formula1>"addgene,genbank,benchling"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1730,7 +1730,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank"</formula1>
+      <formula1>"addgene,genbank,benchling"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1804,7 +1804,7 @@
       <formula1>"depositor-full,addgene-full"</formula1>
     </dataValidation>
     <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank"</formula1>
+      <formula1>"addgene,genbank,benchling"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
new PCR model for https://github.com/manulera/ShareYourCloning_backend/issues/159
</commit_message>
<xml_diff>
--- a/project/excel/shareyourcloning_linkml.xlsx
+++ b/project/excel/shareyourcloning_linkml.xlsx
@@ -877,56 +877,46 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>forward_primer</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>reverse_primer</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
         <is>
           <t>circular</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>assembly</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>input</t>
+          <t>type</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>output</t>
+          <t>output_name</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
         <is>
           <t>id</t>
         </is>

</xml_diff>

<commit_message>
New pcr model (#12)
* new PCR model for https://github.com/manulera/ShareYourCloning_backend/issues/159

* remove input cardinality constrains
</commit_message>
<xml_diff>
--- a/project/excel/shareyourcloning_linkml.xlsx
+++ b/project/excel/shareyourcloning_linkml.xlsx
@@ -877,56 +877,46 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>forward_primer</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>reverse_primer</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
         <is>
           <t>circular</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>assembly</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>input</t>
+          <t>type</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>output</t>
+          <t>output_name</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
         <is>
           <t>id</t>
         </is>

</xml_diff>

<commit_message>
update to next linkML
</commit_message>
<xml_diff>
--- a/project/excel/shareyourcloning_linkml.xlsx
+++ b/project/excel/shareyourcloning_linkml.xlsx
@@ -1,39 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TextFileSequence" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Primer" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SequenceCut" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RestrictionSequenceCut" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ManuallyTypedSource" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UploadedFileSource" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RepositoryIdSource" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AddGeneIdSource" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BenchlingUrlSource" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GenomeCoordinatesSource" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SequenceCutSource" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RestrictionEnzymeDigestionSource" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SimpleSequenceLocation" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AssemblyJoinComponent" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AssemblyJoin" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AssemblySource" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PCRSource" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LigationSource" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HomologousRecombinationSource" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GibsonAssemblySource" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="OverlapExtensionPCRLigationSource" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RestrictionAndLigationSource" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CRISPRSource" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="OligoHybridizationSource" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PolymeraseExtensionSource" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CloningStrategy" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="TextFileSequence" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Primer" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="SequenceCut" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="RestrictionSequenceCut" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="ManuallyTypedSource" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="UploadedFileSource" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="RepositoryIdSource" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="AddGeneIdSource" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="BenchlingUrlSource" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="GenomeCoordinatesSource" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="SequenceCutSource" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="RestrictionEnzymeDigestionSource" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="SimpleSequenceLocation" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="AssemblyJoinComponent" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="AssemblyJoin" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="AssemblySource" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="PCRSource" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="LigationSource" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="HomologousRecombinationSource" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="GibsonAssemblySource" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="OverlapExtensionPCRLigationSource" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="RestrictionAndLigationSource" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="CRISPRSource" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="OligoHybridizationSource" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="PolymeraseExtensionSource" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="CloningStrategy" sheetId="27" state="visible" r:id="rId27"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
first step towards #7
</commit_message>
<xml_diff>
--- a/project/excel/shareyourcloning_linkml.xlsx
+++ b/project/excel/shareyourcloning_linkml.xlsx
@@ -21,19 +21,18 @@
     <sheet name="SequenceCutSource" sheetId="12" state="visible" r:id="rId12"/>
     <sheet name="RestrictionEnzymeDigestionSource" sheetId="13" state="visible" r:id="rId13"/>
     <sheet name="SimpleSequenceLocation" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="AssemblyJoinComponent" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="AssemblyJoin" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="AssemblySource" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="PCRSource" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="LigationSource" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="HomologousRecombinationSource" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="GibsonAssemblySource" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="OverlapExtensionPCRLigationSource" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="RestrictionAndLigationSource" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="CRISPRSource" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="OligoHybridizationSource" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="PolymeraseExtensionSource" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="CloningStrategy" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="AssemblyFragment" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="AssemblySource" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="PCRSource" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="LigationSource" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="HomologousRecombinationSource" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="GibsonAssemblySource" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="OverlapExtensionPCRLigationSource" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="RestrictionAndLigationSource" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="CRISPRSource" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="OligoHybridizationSource" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="PolymeraseExtensionSource" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="CloningStrategy" sheetId="26" state="visible" r:id="rId26"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -476,14 +475,14 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>repository_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>repository_name</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>repository_id</t>
-        </is>
-      </c>
       <c r="C1" t="inlineStr">
         <is>
           <t>input</t>
@@ -512,7 +511,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"addgene,genbank,benchling"</formula1>
     </dataValidation>
   </dataValidations>
@@ -755,7 +754,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -771,10 +770,15 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>location</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
+          <t>left_location</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>right_location</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
         <is>
           <t>reverse_complemented</t>
         </is>
@@ -791,23 +795,48 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>left</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>right</t>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>assembly</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
         </is>
       </c>
     </row>
@@ -1158,230 +1187,220 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>restriction_enzymes</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
         <is>
           <t>circular</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>assembly</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>input</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>output</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>guides</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>assembly</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>type</t>
+          <t>output</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>output_name</t>
         </is>
       </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>overhang_crick_3prime</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>forward_oligo</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>reverse_oligo</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>restriction_enzymes</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>circular</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>assembly</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
         <is>
           <t>input</t>
         </is>
       </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>guides</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>circular</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>assembly</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>overhang_crick_3prime</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>forward_oligo</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>reverse_oligo</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
           <t>id</t>
         </is>
       </c>
@@ -1392,52 +1411,6 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1740,14 +1713,14 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>repository_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>repository_name</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>repository_id</t>
-        </is>
-      </c>
       <c r="C1" t="inlineStr">
         <is>
           <t>input</t>
@@ -1776,7 +1749,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"addgene,genbank,benchling"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1811,12 +1784,12 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>repository_id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>repository_name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>repository_id</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -1850,7 +1823,7 @@
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"depositor-full,addgene-full"</formula1>
     </dataValidation>
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"addgene,genbank,benchling"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Revert "add SnapGene library"
This reverts commit 894c07f1c2cbb019f7a12b8a22f157ac7969f279.
</commit_message>
<xml_diff>
--- a/project/excel/shareyourcloning_linkml.xlsx
+++ b/project/excel/shareyourcloning_linkml.xlsx
@@ -1,40 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="TextFileSequence" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Primer" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="SequenceCut" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="RestrictionSequenceCut" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="ManuallyTypedSource" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="UploadedFileSource" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="RepositoryIdSource" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="AddGeneIdSource" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="BenchlingUrlSource" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="SnapGenePlasmidSource" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="GenomeCoordinatesSource" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="SequenceCutSource" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="RestrictionEnzymeDigestionSource" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="SimpleSequenceLocation" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="AssemblyJoinComponent" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="AssemblyJoin" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="AssemblySource" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="PCRSource" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="LigationSource" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="HomologousRecombinationSource" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="GibsonAssemblySource" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="OverlapExtensionPCRLigationSource" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="RestrictionAndLigationSource" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="CRISPRSource" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="OligoHybridizationSource" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="PolymeraseExtensionSource" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="CloningStrategy" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TextFileSequence" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Primer" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SequenceCut" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RestrictionSequenceCut" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ManuallyTypedSource" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UploadedFileSource" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RepositoryIdSource" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AddGeneIdSource" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BenchlingUrlSource" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GenomeCoordinatesSource" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SequenceCutSource" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RestrictionEnzymeDigestionSource" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SimpleSequenceLocation" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AssemblyJoinComponent" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AssemblyJoin" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AssemblySource" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PCRSource" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LigationSource" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HomologousRecombinationSource" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GibsonAssemblySource" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="OverlapExtensionPCRLigationSource" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RestrictionAndLigationSource" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CRISPRSource" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="OligoHybridizationSource" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PolymeraseExtensionSource" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CloningStrategy" sheetId="27" state="visible" r:id="rId27"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -527,6 +526,87 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>assembly_accession</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sequence_accession</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>locus_tag</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>gene_id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>start</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>end</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>strand</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -538,12 +618,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>repository_name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>repository_id</t>
+          <t>left_edge</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>right_edge</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -573,303 +653,217 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>assembly_accession</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sequence_accession</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>locus_tag</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>gene_id</t>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>left_edge</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>right_edge</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>start</t>
         </is>
       </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>end</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>strand</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sequence</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>location</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>reverse_complemented</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>right</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>assembly</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>end</t>
+          <t>output_name</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>strand</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>left_edge</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>right_edge</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>left_edge</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>right_edge</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>start</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>end</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>strand</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sequence</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>location</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>reverse_complemented</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>left</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>right</t>
+          <t>id</t>
         </is>
       </c>
     </row>
@@ -1220,230 +1214,220 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>restriction_enzymes</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
         <is>
           <t>circular</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>assembly</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>input</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>output</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>guides</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>assembly</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>type</t>
+          <t>output</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>output_name</t>
         </is>
       </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>overhang_crick_3prime</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>forward_oligo</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>reverse_oligo</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>restriction_enzymes</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>circular</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>assembly</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
         <is>
           <t>input</t>
         </is>
       </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>guides</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>circular</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>assembly</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>overhang_crick_3prime</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>forward_oligo</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>reverse_oligo</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
           <t>id</t>
         </is>
       </c>
@@ -1454,52 +1438,6 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
Issue 7 2 (#15)
* update to next linkML

* first step towards #7

* make left_location and right_location nullable
</commit_message>
<xml_diff>
--- a/project/excel/shareyourcloning_linkml.xlsx
+++ b/project/excel/shareyourcloning_linkml.xlsx
@@ -1,39 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TextFileSequence" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Primer" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SequenceCut" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RestrictionSequenceCut" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ManuallyTypedSource" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UploadedFileSource" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RepositoryIdSource" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AddGeneIdSource" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BenchlingUrlSource" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GenomeCoordinatesSource" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SequenceCutSource" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RestrictionEnzymeDigestionSource" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SimpleSequenceLocation" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AssemblyJoinComponent" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AssemblyJoin" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AssemblySource" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PCRSource" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LigationSource" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HomologousRecombinationSource" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GibsonAssemblySource" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="OverlapExtensionPCRLigationSource" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RestrictionAndLigationSource" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CRISPRSource" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="OligoHybridizationSource" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PolymeraseExtensionSource" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CloningStrategy" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="TextFileSequence" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Primer" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="SequenceCut" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="RestrictionSequenceCut" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="ManuallyTypedSource" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="UploadedFileSource" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="RepositoryIdSource" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="AddGeneIdSource" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="BenchlingUrlSource" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="GenomeCoordinatesSource" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="SequenceCutSource" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="RestrictionEnzymeDigestionSource" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="SimpleSequenceLocation" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="AssemblyFragment" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="AssemblySource" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="PCRSource" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="LigationSource" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="HomologousRecombinationSource" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="GibsonAssemblySource" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="OverlapExtensionPCRLigationSource" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="RestrictionAndLigationSource" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="CRISPRSource" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="OligoHybridizationSource" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="PolymeraseExtensionSource" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="CloningStrategy" sheetId="26" state="visible" r:id="rId26"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -476,14 +475,14 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>repository_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>repository_name</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>repository_id</t>
-        </is>
-      </c>
       <c r="C1" t="inlineStr">
         <is>
           <t>input</t>
@@ -512,7 +511,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"addgene,genbank,benchling"</formula1>
     </dataValidation>
   </dataValidations>
@@ -755,7 +754,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -771,10 +770,15 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>location</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
+          <t>left_location</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>right_location</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
         <is>
           <t>reverse_complemented</t>
         </is>
@@ -791,23 +795,48 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>left</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>right</t>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>assembly</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
         </is>
       </c>
     </row>
@@ -1158,230 +1187,220 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>restriction_enzymes</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
         <is>
           <t>circular</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>assembly</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>input</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>output</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>guides</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>assembly</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>type</t>
+          <t>output</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>output_name</t>
         </is>
       </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>overhang_crick_3prime</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>forward_oligo</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>reverse_oligo</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>restriction_enzymes</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>circular</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>assembly</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
         <is>
           <t>input</t>
         </is>
       </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>guides</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>circular</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>assembly</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>overhang_crick_3prime</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>forward_oligo</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>reverse_oligo</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
           <t>id</t>
         </is>
       </c>
@@ -1392,52 +1411,6 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1740,14 +1713,14 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>repository_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>repository_name</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>repository_id</t>
-        </is>
-      </c>
       <c r="C1" t="inlineStr">
         <is>
           <t>input</t>
@@ -1776,7 +1749,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"addgene,genbank,benchling"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1811,12 +1784,12 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>repository_id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>repository_name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>repository_id</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -1850,7 +1823,7 @@
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"depositor-full,addgene-full"</formula1>
     </dataValidation>
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"addgene,genbank,benchling"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
add SnapGene library 2 (#17)
* update test files

* add SnapGene library
</commit_message>
<xml_diff>
--- a/project/excel/shareyourcloning_linkml.xlsx
+++ b/project/excel/shareyourcloning_linkml.xlsx
@@ -17,22 +17,23 @@
     <sheet name="RepositoryIdSource" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="AddGeneIdSource" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="BenchlingUrlSource" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="GenomeCoordinatesSource" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="SequenceCutSource" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="RestrictionEnzymeDigestionSource" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="SimpleSequenceLocation" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="AssemblyFragment" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="AssemblySource" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="PCRSource" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="LigationSource" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="HomologousRecombinationSource" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="GibsonAssemblySource" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="OverlapExtensionPCRLigationSource" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="RestrictionAndLigationSource" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="CRISPRSource" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="OligoHybridizationSource" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="PolymeraseExtensionSource" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="CloningStrategy" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="SnapGenePlasmidSource" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="GenomeCoordinatesSource" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="SequenceCutSource" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="RestrictionEnzymeDigestionSource" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="SimpleSequenceLocation" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="AssemblyFragment" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="AssemblySource" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="PCRSource" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="LigationSource" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="HomologousRecombinationSource" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="GibsonAssemblySource" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="OverlapExtensionPCRLigationSource" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="RestrictionAndLigationSource" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="CRISPRSource" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="OligoHybridizationSource" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="PolymeraseExtensionSource" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="CloningStrategy" sheetId="27" state="visible" r:id="rId27"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -525,6 +526,67 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>repository_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>repository_name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"addgene,genbank,benchling"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -600,7 +662,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -656,7 +718,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -712,7 +774,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -748,7 +810,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -781,62 +843,6 @@
       <c r="D1" t="inlineStr">
         <is>
           <t>reverse_complemented</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>circular</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>assembly</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>id</t>
         </is>
       </c>
     </row>
@@ -1187,6 +1193,62 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>assembly</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1242,7 +1304,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1303,7 +1365,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1364,7 +1426,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1410,7 +1472,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
add missing enum element
</commit_message>
<xml_diff>
--- a/project/excel/shareyourcloning_linkml.xlsx
+++ b/project/excel/shareyourcloning_linkml.xlsx
@@ -513,7 +513,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -574,7 +574,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1812,7 +1812,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1886,7 +1886,7 @@
       <formula1>"depositor-full,addgene-full"</formula1>
     </dataValidation>
     <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add missing enum element (#18)
</commit_message>
<xml_diff>
--- a/project/excel/shareyourcloning_linkml.xlsx
+++ b/project/excel/shareyourcloning_linkml.xlsx
@@ -513,7 +513,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -574,7 +574,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1812,7 +1812,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1886,7 +1886,7 @@
       <formula1>"depositor-full,addgene-full"</formula1>
     </dataValidation>
     <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
support for euroscarf (#19)
</commit_message>
<xml_diff>
--- a/project/excel/shareyourcloning_linkml.xlsx
+++ b/project/excel/shareyourcloning_linkml.xlsx
@@ -18,22 +18,23 @@
     <sheet name="AddGeneIdSource" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="BenchlingUrlSource" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="SnapGenePlasmidSource" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="GenomeCoordinatesSource" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="SequenceCutSource" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="RestrictionEnzymeDigestionSource" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="SimpleSequenceLocation" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="AssemblyFragment" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="AssemblySource" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="PCRSource" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="LigationSource" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="HomologousRecombinationSource" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="GibsonAssemblySource" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="OverlapExtensionPCRLigationSource" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="RestrictionAndLigationSource" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="CRISPRSource" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="OligoHybridizationSource" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="PolymeraseExtensionSource" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="CloningStrategy" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="EuroscarfSource" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="GenomeCoordinatesSource" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="SequenceCutSource" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="RestrictionEnzymeDigestionSource" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="SimpleSequenceLocation" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="AssemblyFragment" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="AssemblySource" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="PCRSource" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="LigationSource" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="HomologousRecombinationSource" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="GibsonAssemblySource" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="OverlapExtensionPCRLigationSource" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="RestrictionAndLigationSource" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="CRISPRSource" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="OligoHybridizationSource" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="PolymeraseExtensionSource" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="CloningStrategy" sheetId="28" state="visible" r:id="rId28"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -513,7 +514,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -574,7 +575,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -587,6 +588,67 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>repository_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>repository_name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -662,7 +724,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -718,7 +780,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -774,7 +836,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -810,7 +872,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -843,62 +905,6 @@
       <c r="D1" t="inlineStr">
         <is>
           <t>reverse_complemented</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>circular</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>assembly</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>id</t>
         </is>
       </c>
     </row>
@@ -1249,6 +1255,62 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>assembly</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1304,7 +1366,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1365,7 +1427,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1426,7 +1488,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1472,7 +1534,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1812,7 +1874,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1886,7 +1948,7 @@
       <formula1>"depositor-full,addgene-full"</formula1>
     </dataValidation>
     <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
gateway cloning for https://github.com/manulera/ShareYourCloning_backend/issues/215
</commit_message>
<xml_diff>
--- a/project/excel/shareyourcloning_linkml.xlsx
+++ b/project/excel/shareyourcloning_linkml.xlsx
@@ -31,10 +31,11 @@
     <sheet name="GibsonAssemblySource" sheetId="22" state="visible" r:id="rId22"/>
     <sheet name="OverlapExtensionPCRLigationSource" sheetId="23" state="visible" r:id="rId23"/>
     <sheet name="RestrictionAndLigationSource" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="CRISPRSource" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="OligoHybridizationSource" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="PolymeraseExtensionSource" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="CloningStrategy" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="GatewaySource" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="CRISPRSource" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="OligoHybridizationSource" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="PolymeraseExtensionSource" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="CloningStrategy" sheetId="29" state="visible" r:id="rId29"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1383,6 +1384,72 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>reaction_type</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>assembly</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"LR,BR"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>guides</t>
         </is>
       </c>
@@ -1427,7 +1494,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1488,7 +1555,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1534,7 +1601,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
add greedy to GatewaySource
</commit_message>
<xml_diff>
--- a/project/excel/shareyourcloning_linkml.xlsx
+++ b/project/excel/shareyourcloning_linkml.xlsx
@@ -1373,7 +1373,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1389,35 +1389,40 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>greedy</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>circular</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>assembly</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>input</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>output</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
       <c r="G1" t="inlineStr">
         <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>output_name</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>id</t>
         </is>

</xml_diff>

<commit_message>
add add_primer_features to primers
</commit_message>
<xml_diff>
--- a/project/excel/shareyourcloning_linkml.xlsx
+++ b/project/excel/shareyourcloning_linkml.xlsx
@@ -976,46 +976,51 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>add_primer_features</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
         <is>
           <t>circular</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>assembly</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>input</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>output</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>output_name</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>id</t>
         </is>

</xml_diff>

<commit_message>
add add_primer_features to primers (#21)
</commit_message>
<xml_diff>
--- a/project/excel/shareyourcloning_linkml.xlsx
+++ b/project/excel/shareyourcloning_linkml.xlsx
@@ -976,46 +976,51 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>add_primer_features</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
         <is>
           <t>circular</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>assembly</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>input</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>output</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>output_name</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>id</t>
         </is>

</xml_diff>

<commit_message>
add type to allow Union of classes
</commit_message>
<xml_diff>
--- a/project/excel/shareyourcloning_linkml.xlsx
+++ b/project/excel/shareyourcloning_linkml.xlsx
@@ -1766,7 +1766,15 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1777,7 +1785,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1854,6 +1862,11 @@
       <c r="N1" t="inlineStr">
         <is>
           <t>sequence</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>type</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
support for iGEM collections https://github.com/manulera/ShareYourCloning_backend/issues/240
</commit_message>
<xml_diff>
--- a/project/excel/shareyourcloning_linkml.xlsx
+++ b/project/excel/shareyourcloning_linkml.xlsx
@@ -19,27 +19,28 @@
     <sheet name="BenchlingUrlSource" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="SnapGenePlasmidSource" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="EuroscarfSource" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="GenomeCoordinatesSource" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="SequenceCutSource" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="RestrictionEnzymeDigestionSource" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="SimpleSequenceLocation" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="AssemblyFragment" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="AssemblySource" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="PCRSource" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="LigationSource" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="HomologousRecombinationSource" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="GibsonAssemblySource" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="InFusionSource" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="OverlapExtensionPCRLigationSource" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="RestrictionAndLigationSource" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="GatewaySource" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="CRISPRSource" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="OligoHybridizationSource" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="PolymeraseExtensionSource" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="CloningStrategy" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="AnnotationReport" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="PlannotateAnnotationReport" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet name="AnnotationSource" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="IGEMSource" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="GenomeCoordinatesSource" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="SequenceCutSource" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="RestrictionEnzymeDigestionSource" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="SimpleSequenceLocation" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="AssemblyFragment" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="AssemblySource" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="PCRSource" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="LigationSource" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="HomologousRecombinationSource" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="GibsonAssemblySource" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="InFusionSource" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="OverlapExtensionPCRLigationSource" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="RestrictionAndLigationSource" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="GatewaySource" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="CRISPRSource" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="OligoHybridizationSource" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="PolymeraseExtensionSource" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="CloningStrategy" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="AnnotationReport" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="PlannotateAnnotationReport" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="AnnotationSource" sheetId="34" state="visible" r:id="rId34"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -654,6 +655,67 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>repository_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>repository_name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -729,7 +791,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -785,7 +847,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -841,7 +903,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -877,7 +939,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -918,7 +980,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -964,67 +1026,6 @@
         </is>
       </c>
       <c r="G1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>add_primer_features</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>circular</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>assembly</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -1097,6 +1098,67 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>add_primer_features</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>assembly</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1147,7 +1209,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1203,7 +1265,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1259,7 +1321,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1315,7 +1377,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1371,7 +1433,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1432,7 +1494,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1503,7 +1565,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1564,7 +1626,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1625,7 +1687,48 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sequence</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1671,7 +1774,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1688,182 +1791,141 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
+          <t>sequences</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sources</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>primers</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sseqid</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>start_location</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>end_location</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>strand</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>percent_identity</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>full_length_of_feature_in_db</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>length_of_found_feature</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>percent_match_length</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>fragment</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>database</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
         <is>
           <t>sequence</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sequences</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sources</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>primers</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:O1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sseqid</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>start_location</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>end_location</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>strand</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>percent_identity</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>full_length_of_feature_in_db</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>length_of_found_feature</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>percent_match_length</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>fragment</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>database</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>Feature</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>Type</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>sequence</t>
-        </is>
-      </c>
       <c r="O1" t="inlineStr">
         <is>
           <t>type</t>
@@ -1875,7 +1937,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
add igem as RepositoryName
</commit_message>
<xml_diff>
--- a/project/excel/shareyourcloning_linkml.xlsx
+++ b/project/excel/shareyourcloning_linkml.xlsx
@@ -520,7 +520,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -581,7 +581,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -642,7 +642,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -708,7 +708,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2266,7 +2266,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2340,7 +2340,7 @@
       <formula1>"depositor-full,addgene-full"</formula1>
     </dataValidation>
     <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
support for iGEM collections  (#24)
* support for iGEM collections https://github.com/manulera/ShareYourCloning_backend/issues/240

* include slot

* add igem as RepositoryName

* make url compulsory

* make url compulsory
</commit_message>
<xml_diff>
--- a/project/excel/shareyourcloning_linkml.xlsx
+++ b/project/excel/shareyourcloning_linkml.xlsx
@@ -19,27 +19,28 @@
     <sheet name="BenchlingUrlSource" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="SnapGenePlasmidSource" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="EuroscarfSource" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="GenomeCoordinatesSource" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="SequenceCutSource" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="RestrictionEnzymeDigestionSource" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="SimpleSequenceLocation" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="AssemblyFragment" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="AssemblySource" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="PCRSource" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="LigationSource" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="HomologousRecombinationSource" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="GibsonAssemblySource" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="InFusionSource" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="OverlapExtensionPCRLigationSource" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="RestrictionAndLigationSource" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="GatewaySource" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="CRISPRSource" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="OligoHybridizationSource" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="PolymeraseExtensionSource" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="CloningStrategy" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="AnnotationReport" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="PlannotateAnnotationReport" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet name="AnnotationSource" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="IGEMSource" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="GenomeCoordinatesSource" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="SequenceCutSource" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="RestrictionEnzymeDigestionSource" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="SimpleSequenceLocation" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="AssemblyFragment" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="AssemblySource" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="PCRSource" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="LigationSource" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="HomologousRecombinationSource" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="GibsonAssemblySource" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="InFusionSource" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="OverlapExtensionPCRLigationSource" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="RestrictionAndLigationSource" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="GatewaySource" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="CRISPRSource" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="OligoHybridizationSource" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="PolymeraseExtensionSource" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="CloningStrategy" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="AnnotationReport" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="PlannotateAnnotationReport" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="AnnotationSource" sheetId="34" state="visible" r:id="rId34"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -519,7 +520,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -580,7 +581,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -641,7 +642,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -654,6 +655,72 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sequence_file_url</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>repository_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>repository_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -729,7 +796,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -785,7 +852,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -841,7 +908,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -877,7 +944,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -918,7 +985,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -964,67 +1031,6 @@
         </is>
       </c>
       <c r="G1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>add_primer_features</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>circular</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>assembly</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -1097,6 +1103,67 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>add_primer_features</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>assembly</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1147,7 +1214,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1203,7 +1270,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1259,7 +1326,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1315,7 +1382,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1371,7 +1438,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1432,7 +1499,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1503,7 +1570,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1564,7 +1631,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1625,7 +1692,48 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sequence</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1671,7 +1779,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1688,182 +1796,141 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
+          <t>sequences</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sources</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>primers</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sseqid</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>start_location</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>end_location</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>strand</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>percent_identity</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>full_length_of_feature_in_db</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>length_of_found_feature</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>percent_match_length</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>fragment</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>database</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
         <is>
           <t>sequence</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sequences</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sources</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>primers</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:O1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sseqid</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>start_location</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>end_location</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>strand</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>percent_identity</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>full_length_of_feature_in_db</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>length_of_found_feature</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>percent_match_length</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>fragment</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>database</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>Feature</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>Type</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>sequence</t>
-        </is>
-      </c>
       <c r="O1" t="inlineStr">
         <is>
           <t>type</t>
@@ -1875,7 +1942,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2199,7 +2266,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2273,7 +2340,7 @@
       <formula1>"depositor-full,addgene-full"</formula1>
     </dataValidation>
     <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>